<commit_message>
update file kien thuc
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\tiktok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424B4BD7-73C5-4897-A1D6-38F7871373ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBFD467-9C45-4D60-BAF2-1F57A99350A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F52B70D0-E6FF-4AE3-AC02-831A36674E1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{F52B70D0-E6FF-4AE3-AC02-831A36674E1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="JS-ES6" sheetId="1" r:id="rId3"/>
     <sheet name="DOM" sheetId="2" r:id="rId4"/>
     <sheet name="ReactJS" sheetId="6" r:id="rId5"/>
-    <sheet name="Props" sheetId="4" r:id="rId6"/>
+    <sheet name="HTTP request ,API,fetch API" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="276">
   <si>
     <t>Enhance oject literial</t>
   </si>
@@ -182,9 +183,6 @@
     <t>Phân biệt:</t>
   </si>
   <si>
-    <t>Props là cái chứa các thuộc tính cho react element</t>
-  </si>
-  <si>
     <t>Truyền thộc tính props hay gặp TH undefined. Do chưa được khởi tạo</t>
   </si>
   <si>
@@ -194,9 +192,6 @@
     <t>Co the su dung destructuring</t>
   </si>
   <si>
-    <t>DOM event :là các sự kiện click ,…</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. SSR </t>
   </si>
   <si>
@@ -759,13 +754,118 @@
   </si>
   <si>
     <t>nó sẽ xác định việc component có re-render lại hay không . Mặc định trả về true ta có thể thay đổi true</t>
+  </si>
+  <si>
+    <t>BẢNG KIỂM ĐIỂM</t>
+  </si>
+  <si>
+    <t>Hà Nội, Ngày 17 -11 -2022</t>
+  </si>
+  <si>
+    <t>Họ tên anh iu</t>
+  </si>
+  <si>
+    <t>Mạnh Lợn</t>
+  </si>
+  <si>
+    <t>Họ tên bé iu</t>
+  </si>
+  <si>
+    <t>Bé Loan</t>
+  </si>
+  <si>
+    <t>Anh làm đơn này để xin lỗi vì những gì a đã gây ra vào tối hôm qua ngày 16-11-2022 . Anh đã cáu bẩn khi em chỉ nói trêu a 1 chút</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anh đã không giữ được bình tĩnh dẫn đến cáu em và làm em buồn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anh rất xin lỗi ! Anh hứa từ sau a khum cáu bẩn và dỗi bé nữa . </t>
+  </si>
+  <si>
+    <t>Người làm đơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anh yêu em!!!! Mong em tha thứ cho anh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hook </t>
+  </si>
+  <si>
+    <t>là các hàm cho phép mình móc vào các trạng thái của React ,và các tính năng vòng đời từ các hàm components</t>
+  </si>
+  <si>
+    <t>Hooks hoạt động k cần class , hoạt động trong function components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nó giúp chúng ta có thể sử dụng state và life cycle trong function components , thay thế được class components </t>
+  </si>
+  <si>
+    <t>useState()</t>
+  </si>
+  <si>
+    <t>useEffect()</t>
+  </si>
+  <si>
+    <t>useLayoutEffect()</t>
+  </si>
+  <si>
+    <t>useRef()</t>
+  </si>
+  <si>
+    <t>useMemo()</t>
+  </si>
+  <si>
+    <t>useCallback()</t>
+  </si>
+  <si>
+    <t>useReducer()</t>
+  </si>
+  <si>
+    <t>useContext()</t>
+  </si>
+  <si>
+    <t>Khi dung thành phần nào sẽ import thành phần đó để gọi</t>
+  </si>
+  <si>
+    <t>useDebugValue()</t>
+  </si>
+  <si>
+    <t>useImperativeHandle()</t>
+  </si>
+  <si>
+    <t>Hooks gồm 10 thành phần:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nó giúp component trở nên đơn giản dễ hiểu hơn </t>
+  </si>
+  <si>
+    <t>trạng thái của dữ liệu , khi chúng ta muốn cập nhật lại dữ liệu và component sẽ tự render lại</t>
+  </si>
+  <si>
+    <t>cách dùng:import vào function component</t>
+  </si>
+  <si>
+    <t>tất cả các hook đều là hàm</t>
+  </si>
+  <si>
+    <t>đối số là : giá trị khởi tạo initState</t>
+  </si>
+  <si>
+    <t>nó trả về 1 mảng 2 phần tử : phần tử 1 là state , phần tử 2 là 1 hàm để set lại state</t>
+  </si>
+  <si>
+    <t>ví dụ: const dulieu [state,setState] = useState[giá trị init]</t>
+  </si>
+  <si>
+    <t>component sẽ được render lại khi setState gọi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,6 +914,31 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1007,7 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1044,6 +1169,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1854,11 +1983,11 @@
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -1871,7 +2000,7 @@
       <c r="L2" s="12"/>
       <c r="M2" s="18"/>
       <c r="Q2" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
@@ -1879,7 +2008,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1899,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -1913,7 +2042,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="18"/>
       <c r="N4" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O4" s="11"/>
     </row>
@@ -1922,7 +2051,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -1939,10 +2068,10 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1950,7 +2079,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -1967,10 +2096,10 @@
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1978,7 +2107,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1997,7 +2126,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -2011,13 +2140,13 @@
       <c r="L8" s="12"/>
       <c r="M8" s="18"/>
       <c r="N8" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2032,7 +2161,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="18"/>
       <c r="O9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2040,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -2059,7 +2188,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -2073,13 +2202,13 @@
       <c r="L11" s="12"/>
       <c r="M11" s="18"/>
       <c r="N11" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -2099,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -2118,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2132,7 +2261,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="18"/>
       <c r="Q14" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R14" s="24"/>
       <c r="S14" s="24"/>
@@ -2143,7 +2272,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -2172,19 +2301,19 @@
       <c r="L16" s="12"/>
       <c r="M16" s="18"/>
       <c r="N16" t="s">
+        <v>92</v>
+      </c>
+      <c r="R16" t="s">
         <v>94</v>
-      </c>
-      <c r="R16" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
@@ -2197,12 +2326,12 @@
       <c r="L17" s="12"/>
       <c r="M17" s="18"/>
       <c r="R17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -2217,15 +2346,15 @@
       <c r="L18" s="12"/>
       <c r="M18" s="18"/>
       <c r="N18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -2240,7 +2369,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="18"/>
       <c r="R19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2248,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -2262,7 +2391,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="18"/>
       <c r="R20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2270,7 +2399,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -2289,7 +2418,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -2308,7 +2437,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -2327,7 +2456,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -2343,7 +2472,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -2363,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
@@ -2382,7 +2511,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -2401,7 +2530,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -2417,7 +2546,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2437,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -2456,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -2510,7 +2639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2185E8-7F78-4A7E-B614-1886F07EB29C}">
   <dimension ref="A2:P94"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2699,222 +2828,222 @@
     </row>
     <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B54" s="1"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D62" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D63" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D65" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
+        <v>118</v>
+      </c>
+      <c r="D67" t="s">
         <v>120</v>
-      </c>
-      <c r="D67" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D69" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A71" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B71" s="1"/>
       <c r="D71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G78" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B84" s="27"/>
       <c r="D84" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D90" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D91" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B94" s="1"/>
     </row>
@@ -2995,10 +3124,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58449254-F20A-40EB-816D-1CE919B5BD7B}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,123 +3138,123 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -3150,309 +3279,418 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E28" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F32" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="F35" s="30" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E35" s="29" t="s">
+      <c r="G35" t="s">
         <v>182</v>
       </c>
-      <c r="F35" s="30" t="s">
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
         <v>183</v>
       </c>
-      <c r="G35" t="s">
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
         <v>50</v>
       </c>
-      <c r="L35" t="s">
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="29" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G36" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G37" t="s">
+      <c r="G42" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E42" s="29" t="s">
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
         <v>186</v>
       </c>
-      <c r="G42" t="s">
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G43" t="s">
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G44" t="s">
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F46" s="30" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G45" t="s">
+      <c r="G46" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F46" s="30" t="s">
+    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
         <v>191</v>
       </c>
-      <c r="G46" t="s">
+    </row>
+    <row r="48" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G47" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G48" t="s">
-        <v>194</v>
-      </c>
       <c r="I48" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G49" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I49" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G51" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="I51" t="s">
         <v>205</v>
-      </c>
-      <c r="I51" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I52" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G53" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I53" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I54" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I56" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G58" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F59" s="30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G59" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E61" s="29" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G61" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F63" s="30" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G63" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G64" s="31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I64" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G66" s="31" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I66" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I68" t="s">
+        <v>222</v>
+      </c>
+      <c r="L68" t="s">
         <v>224</v>
-      </c>
-      <c r="L68" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="69" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L69" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="70" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I70" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L70" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L71" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G72" s="31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I72" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I73" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L74" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I76" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L76" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" spans="7:12" x14ac:dyDescent="0.25">
       <c r="I77" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L77" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G78" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I78" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L78" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L79" t="s">
-        <v>241</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E82" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="F82" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="83" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="85" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>267</v>
+      </c>
+      <c r="H86" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="J86" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>271</v>
+      </c>
+      <c r="J87" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="90" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="100" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="101" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="103" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="104" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="105" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="106" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3462,22 +3700,307 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F0FBEE-5633-4D6E-B6E4-7A2A92C8C983}">
-  <dimension ref="A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EBB855-2665-4FC7-B0F7-F614BC4905D7}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A272810-FAA8-40BC-A59C-D91553439282}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add cau hinh header
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\tiktok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReactJs\tiktok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351CC01F-49EA-4556-A6C8-E1539F353321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB2CAD4-4138-4230-BEB9-D3EB7AA51302}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F52B70D0-E6FF-4AE3-AC02-831A36674E1F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="380">
   <si>
     <t>Enhance oject literial</t>
   </si>
@@ -1088,6 +1088,96 @@
   </si>
   <si>
     <t>Cách bước theo ảnh mình họa:</t>
+  </si>
+  <si>
+    <t>Chỉ gọi hooks at the top level . Không gọi trong vòng lặp,điều kiện ,nested funtion</t>
+  </si>
+  <si>
+    <t>Redux</t>
+  </si>
+  <si>
+    <t>Là 1 thư viện JS dùng để quản lý và cập nhật state của ứng dụng</t>
+  </si>
+  <si>
+    <t>nó như 1 kho trung để quản lý tập trung các state</t>
+  </si>
+  <si>
+    <t>Là một parttern</t>
+  </si>
+  <si>
+    <t>Redux giúp quản lý global state - các components tại mọi nơi trong ứng dụng đều có thể truy xuất và cập nhật</t>
+  </si>
+  <si>
+    <t>Giúp việc truyền dữ liệu vào các cấp component con cháu khác nhau nhanh hơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dễ dàng debug </t>
+  </si>
+  <si>
+    <t>Redux toolkit giải quyết các vấn đề với redux core đó là cấu hình redux phức tạp,cài đặt thủ công nhiều package, tránh viết lại các đoạn code lặp đi lặp lại</t>
+  </si>
+  <si>
+    <t>Kiến trúc của redux</t>
+  </si>
+  <si>
+    <t>Các thành phần của redux</t>
+  </si>
+  <si>
+    <t>Reducer</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Dispatch</t>
+  </si>
+  <si>
+    <t>Là 1 function nó nhận 2 tham số là state cũ có giá trị khởi tạo và 1 action</t>
+  </si>
+  <si>
+    <t>Các quy tắc với reducer: state mới luôn được tính toán dựa trên giá trị state cũ và action</t>
+  </si>
+  <si>
+    <t>Không được thay đổi trực tiếp giá trị state hiện tại mà phải tạo ra bản copy</t>
+  </si>
+  <si>
+    <t>Không được code bất đồng bộ trong reducer (ramdom, date.now, call API,..)</t>
+  </si>
+  <si>
+    <t>Là một object do chúng ta quy định</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type phải có , payload có hoặc không </t>
+  </si>
+  <si>
+    <t>reducer sẽ dựa vào type , nếu muốn state tính toán dựa trên payload truyền vào thì mới khai báo payload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action creators là 1 hàm </t>
+  </si>
+  <si>
+    <t>Là một function  để update state trên store</t>
+  </si>
+  <si>
+    <t>sử dụng hàm dispatch(tham số là action truyền vào)</t>
+  </si>
+  <si>
+    <t>action truyền vào có thể là 1 action creators</t>
+  </si>
+  <si>
+    <t>Quy trình chạy của redux hoạt động:</t>
+  </si>
+  <si>
+    <t>khi 1 sự kiện gì đó dk xảy ra thì eventHandle sẽ được thực thi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gọi đến function dispatch(nhận vào function) sẽ chuyển action đó vào Store . </t>
+  </si>
+  <si>
+    <t>nó sẽ lấy state hiện tại và action vừa được dispatch  truyền vào reducer . Nó sẽ cập nhật trong reducer</t>
+  </si>
+  <si>
+    <t>&gt; UI nhận được thông tin update state sẽ render lại UI</t>
   </si>
 </sst>
 </file>
@@ -1745,6 +1835,99 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>512501</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>86398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B9FD1F-2BC4-4011-8DBA-D3CB1A6C9E2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10887075" y="20545425"/>
+          <a:ext cx="2731826" cy="2229523"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>471731</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>57287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{544A63F2-452B-4E8F-9B35-9BC01E9908C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8667751" y="24260174"/>
+          <a:ext cx="1862380" cy="771663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>55</xdr:row>
@@ -3405,10 +3588,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58449254-F20A-40EB-816D-1CE919B5BD7B}">
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="K93" sqref="K93"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="I123" sqref="I123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3887,96 +4070,232 @@
     </row>
     <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
         <v>267</v>
       </c>
-      <c r="H86" s="31" t="s">
+      <c r="H88" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J88" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="F87" t="s">
+    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
         <v>271</v>
       </c>
-      <c r="J87" t="s">
+      <c r="J89" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J88" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J89" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="J90" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="91" spans="5:10" x14ac:dyDescent="0.25">
       <c r="J91" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H97" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H98" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="99" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H99" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H100" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H101" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H102" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H103" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H104" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="105" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H105" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="106" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="107" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="106" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F106" t="s">
+    <row r="108" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="113" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E113" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F113" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="114" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="115" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="117" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F117" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="118" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F118" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="119" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F119" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="121" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="122" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="124" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F124" t="s">
+        <v>360</v>
+      </c>
+      <c r="G124" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="H124" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="125" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="126" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="127" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="128" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="G128" s="31" t="s">
+        <v>362</v>
+      </c>
+      <c r="H128" t="s">
+        <v>368</v>
+      </c>
+      <c r="O128" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="129" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>371</v>
+      </c>
+      <c r="O129" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="133" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G133" s="31" t="s">
+        <v>363</v>
+      </c>
+      <c r="H133" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="134" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>373</v>
+      </c>
+      <c r="M134" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="136" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G136" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="H136" s="31"/>
+      <c r="I136" s="31"/>
+      <c r="J136" s="31"/>
+      <c r="K136" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="137" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="K137" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="138" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="K138" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="139" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="K139" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
logic phan header-call api
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReactJs\tiktok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB2CAD4-4138-4230-BEB9-D3EB7AA51302}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03D8E2D-EC2D-494D-8849-8084379DC72C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F52B70D0-E6FF-4AE3-AC02-831A36674E1F}"/>
   </bookViews>
@@ -3590,8 +3590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58449254-F20A-40EB-816D-1CE919B5BD7B}">
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="I123" sqref="I123"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="K91" sqref="K91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
use prop-type,fix rename thu muc
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReactJs\tiktok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4D3EF3-9181-4D97-B420-3D03782D57B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645FC5F0-923F-4265-A959-569E7128A4AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{F52B70D0-E6FF-4AE3-AC02-831A36674E1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{F52B70D0-E6FF-4AE3-AC02-831A36674E1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="398">
   <si>
     <t>Enhance oject literial</t>
   </si>
@@ -1227,6 +1227,12 @@
   </si>
   <si>
     <t>cài đặt bằng lệnh npm install axios</t>
+  </si>
+  <si>
+    <t>Props type</t>
+  </si>
+  <si>
+    <t>Dung da validate du lieu</t>
   </si>
 </sst>
 </file>
@@ -3642,7 +3648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58449254-F20A-40EB-816D-1CE919B5BD7B}">
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection activeCell="K91" sqref="K91"/>
     </sheetView>
   </sheetViews>
@@ -4353,10 +4359,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EBB855-2665-4FC7-B0F7-F614BC4905D7}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,37 +4762,37 @@
         <v>384</v>
       </c>
     </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D88" s="10" t="s">
         <v>393</v>
       </c>
@@ -4794,9 +4800,17 @@
         <v>395</v>
       </c>
     </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D90" s="10" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>396</v>
+      </c>
+      <c r="D93" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>